<commit_message>
finished biofuel refactoring, testing started but wrong MFSP computation. Update of calibration excel
</commit_message>
<xml_diff>
--- a/aeromaps/resources/cost_data/Biomass_Data.xlsx
+++ b/aeromaps/resources/cost_data/Biomass_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.salgas.ISAE-SUPAERO\PycharmProjects\AeroMAPS\aeromaps\resources\cost_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E94C87-5EBC-4031-9A92-943A1A0559BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6AB17BA-9190-4321-87B2-02C6A5FC3536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-75" windowWidth="29040" windowHeight="15840" firstSheet="6" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3677,7 +3677,7 @@
     <xf numFmtId="44" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="605">
+  <cellXfs count="607">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -5156,6 +5156,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -7567,8 +7573,8 @@
   </sheetPr>
   <dimension ref="A1:L89"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView topLeftCell="A33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57:D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9343,15 +9349,15 @@
       <c r="A57" s="186" t="s">
         <v>846</v>
       </c>
-      <c r="B57" s="203">
+      <c r="B57" s="605">
         <f>+_xlfn.QUARTILE.EXC(($I$23:$I$24,$I$27,$I$29:$I$45),1)</f>
         <v>2.3297664827195284E-2</v>
       </c>
-      <c r="C57" s="203">
+      <c r="C57" s="605">
         <f>+_xlfn.QUARTILE.EXC(($I$23:$I$24,$I$27,$I$29:$I$45),2)</f>
         <v>3.2956967218057166E-2</v>
       </c>
-      <c r="D57" s="203">
+      <c r="D57" s="605">
         <f>+_xlfn.QUARTILE.EXC(($I$23:$I$24,$I$27,$I$29:$I$45),3)</f>
         <v>4.3672728520463493E-2</v>
       </c>
@@ -9370,15 +9376,15 @@
       <c r="A58" s="189" t="s">
         <v>588</v>
       </c>
-      <c r="B58" s="204">
+      <c r="B58" s="606">
         <f>_xlfn.QUARTILE.EXC(($I$25:$I$26,$I$28),1)</f>
         <v>0</v>
       </c>
-      <c r="C58" s="204">
+      <c r="C58" s="606">
         <f>_xlfn.QUARTILE.EXC(($I$25:$I$26,$I$28),2)</f>
         <v>0</v>
       </c>
-      <c r="D58" s="204">
+      <c r="D58" s="606">
         <f>_xlfn.QUARTILE.EXC(($I$25:$I$26,$I$28),3)</f>
         <v>4.3630973149787994E-5</v>
       </c>
@@ -10068,8 +10074,8 @@
   </sheetPr>
   <dimension ref="A1:N73"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48:G50"/>
+    <sheetView topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14429,8 +14435,8 @@
   </sheetPr>
   <dimension ref="A1:L73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J48" sqref="J48"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added tpdNB and update of excels
</commit_message>
<xml_diff>
--- a/aeromaps/resources/cost_data/Biomass_Data.xlsx
+++ b/aeromaps/resources/cost_data/Biomass_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.salgas.ISAE-SUPAERO\PycharmProjects\AeroMAPS\aeromaps\resources\cost_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42BC2082-2AE4-497D-8F38-B3E3BD44B875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD06E24-89FA-473A-810A-75A8AA07691C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Synthesis" sheetId="1" r:id="rId1"/>
@@ -25,15 +25,15 @@
     <sheet name="Cost Analysis-FT" sheetId="11" r:id="rId10"/>
     <sheet name="Cost Analysis-HEFA" sheetId="9" r:id="rId11"/>
     <sheet name="Cost Summary-V2" sheetId="15" r:id="rId12"/>
-    <sheet name="Feuil1" sheetId="16" r:id="rId13"/>
+    <sheet name="Cost Summary_OLD" sheetId="16" r:id="rId13"/>
     <sheet name="Cost Analysis-AtJ" sheetId="10" r:id="rId14"/>
     <sheet name="Emission factors" sheetId="4" r:id="rId15"/>
     <sheet name="References" sheetId="3" r:id="rId16"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Biomass_Cost!$A$1:$AA$89</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'Cost Summary_OLD'!$A$1:$F$37</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Cost Summary-V1'!$B$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">Feuil1!$A$1:$F$37</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -7577,8 +7577,8 @@
   </sheetPr>
   <dimension ref="A1:L89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29:F37"/>
+    <sheetView topLeftCell="A39" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10078,8 +10078,8 @@
   </sheetPr>
   <dimension ref="A1:N73"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10834,7 +10834,7 @@
         <v>HEFA-Energy</v>
       </c>
       <c r="I26" s="390">
-        <f t="shared" ref="I25:I26" si="0">D26*($F$6*$B$6)/35.3</f>
+        <f t="shared" ref="I26" si="0">D26*($F$6*$B$6)/35.3</f>
         <v>1.4981078709493088E-2</v>
       </c>
       <c r="J26" s="141"/>
@@ -12203,7 +12203,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B407434D-5E27-49A6-8866-38EA42DF7399}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -13196,7 +13196,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A3A65D3-E175-49C7-9833-8199C2B6DD97}">
   <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
@@ -14439,7 +14439,7 @@
   </sheetPr>
   <dimension ref="A1:L73"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
@@ -24973,8 +24973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AFC6162-E2E4-4169-BA68-9742298357E2}">
   <dimension ref="A1:AA94"/>
   <sheetViews>
-    <sheetView topLeftCell="G58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Z61" sqref="Z61"/>
+    <sheetView topLeftCell="G20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Z27" sqref="Z27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31334,7 +31334,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C27A3ECD-44E6-42FD-BAEE-4312D5C51D83}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
@@ -31803,9 +31803,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E83F487-514C-4D2F-B4B9-EA93E171C48F}">
   <dimension ref="A1:M1377"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="L73" sqref="L73"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>